<commit_message>
1.修改spring security passwordEncoder 加密为BCryptPasswordEncoder 2.直接使用UserDetailService 的默认实现 3.更新实体、mapper等
</commit_message>
<xml_diff>
--- a/doc/青柠记账-表设计.xlsx
+++ b/doc/青柠记账-表设计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiesu/IdeaProjects/QingNing/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0E2EA2-3E1A-BA4D-95FA-0272A8AFECC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9930BA93-D326-F143-B120-57114E23C7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="500" windowWidth="24940" windowHeight="14120" xr2:uid="{F5867528-E7AA-634C-AD72-86699A589602}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{F5867528-E7AA-634C-AD72-86699A589602}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
   <si>
     <t>base_table</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,23 +260,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tinyint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>删除标志，默认未删除</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注册时绑定手机号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>账户id，允许字母，数字下划线</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>绑定邮箱，注册时使用account_id进行占位进行占位</t>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UK,逻辑处理保持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绑定邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除标志，默认0未删除,时间戳表示删除时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -642,6 +650,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -660,82 +731,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1054,81 +1062,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877F1F3E-5CD8-E743-BF89-CED463FCFE35}">
   <dimension ref="B2:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="127" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="20.5" style="13" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="16" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="16"/>
+    <col min="2" max="2" width="20.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="10" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="10"/>
     <col min="7" max="7" width="24" customWidth="1"/>
     <col min="9" max="9" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:9">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="17" thickBot="1"/>
     <row r="9" spans="2:9" ht="17" thickTop="1">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="24" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="36"/>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="14" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1137,24 +1145,24 @@
       <c r="H10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="14">
         <v>0</v>
       </c>
-      <c r="E11" s="20" t="b">
+      <c r="E11" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1166,17 +1174,17 @@
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20" t="b">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="1"/>
@@ -1186,15 +1194,15 @@
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
@@ -1202,37 +1210,37 @@
       </c>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33" t="s">
+      <c r="C14" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="22">
         <v>0</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="36" t="s">
-        <v>57</v>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="25" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="17" thickBot="1">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="15">
         <v>0</v>
       </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21">
+      <c r="E15" s="15"/>
+      <c r="F15" s="15">
         <v>0</v>
       </c>
       <c r="G15" s="3"/>
@@ -1243,39 +1251,39 @@
     </row>
     <row r="16" spans="2:9" ht="17" thickTop="1"/>
     <row r="19" spans="2:9">
-      <c r="H19" s="23"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="2:9" ht="17" thickBot="1"/>
     <row r="21" spans="2:9" ht="17" thickTop="1">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I22" s="2" t="s">
@@ -1283,79 +1291,79 @@
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="14"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="11"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="14"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="11"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="2:9">
-      <c r="B25" s="14"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="11"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="2:9" ht="17" thickBot="1">
-      <c r="B26" s="15"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="2:9" ht="17" thickTop="1"/>
     <row r="46" spans="2:9" ht="17" thickBot="1"/>
     <row r="47" spans="2:9" ht="17" thickTop="1">
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="10"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
     </row>
     <row r="48" spans="2:9">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F48" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I48" s="2" t="s">
@@ -1363,80 +1371,80 @@
       </c>
     </row>
     <row r="49" spans="2:9">
-      <c r="B49" s="14"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="11"/>
+      <c r="H49" s="5"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="2:9">
-      <c r="B50" s="14"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="11"/>
+      <c r="H50" s="5"/>
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="2:9">
-      <c r="B51" s="14"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="11"/>
+      <c r="H51" s="5"/>
       <c r="I51" s="2"/>
     </row>
     <row r="52" spans="2:9" ht="17" thickBot="1">
-      <c r="B52" s="15"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="12"/>
+      <c r="H52" s="6"/>
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="2:9" ht="18" thickTop="1" thickBot="1"/>
     <row r="54" spans="2:9" ht="17" thickTop="1">
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="8" t="s">
+      <c r="C54" s="27"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="10"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="31"/>
     </row>
     <row r="55" spans="2:9">
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="18" t="s">
+      <c r="C55" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E55" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F55" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H55" s="11" t="s">
+      <c r="H55" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I55" s="2" t="s">
@@ -1444,134 +1452,134 @@
       </c>
     </row>
     <row r="56" spans="2:9">
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="20">
+      <c r="D56" s="14">
         <v>10</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E56" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="20"/>
+      <c r="F56" s="14"/>
       <c r="G56" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H56" s="11"/>
+      <c r="H56" s="5"/>
       <c r="I56" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="14">
+        <v>32</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="B58" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="14">
+        <v>30</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F58" s="14"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I58" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
-      <c r="B57" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D57" s="20">
-        <v>32</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="2:9">
-      <c r="B58" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" s="20">
-        <v>30</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" s="20"/>
-      <c r="G58" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H58" s="11"/>
-      <c r="I58" s="2" t="s">
+    <row r="59" spans="2:9">
+      <c r="B59" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="22">
+        <v>13</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F59" s="22"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I59" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
-      <c r="B59" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="D59" s="33">
-        <v>13</v>
-      </c>
-      <c r="E59" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="33"/>
-      <c r="G59" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="H59" s="35"/>
-      <c r="I59" s="36" t="s">
-        <v>58</v>
-      </c>
-    </row>
     <row r="60" spans="2:9" ht="17" thickBot="1">
-      <c r="B60" s="15"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
       <c r="G60" s="3"/>
-      <c r="H60" s="12"/>
+      <c r="H60" s="6"/>
       <c r="I60" s="4"/>
     </row>
     <row r="61" spans="2:9" ht="18" thickTop="1" thickBot="1"/>
     <row r="62" spans="2:9" ht="17" thickTop="1">
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="8" t="s">
+      <c r="C62" s="27"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="10"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="31"/>
     </row>
     <row r="63" spans="2:9">
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="18" t="s">
+      <c r="C63" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D63" s="20" t="s">
+      <c r="D63" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E63" s="20" t="s">
+      <c r="E63" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H63" s="11" t="s">
+      <c r="H63" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I63" s="2" t="s">
@@ -1579,103 +1587,103 @@
       </c>
     </row>
     <row r="64" spans="2:9">
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D64" s="20">
+      <c r="D64" s="14">
         <v>10</v>
       </c>
-      <c r="E64" s="20" t="s">
+      <c r="E64" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F64" s="20"/>
+      <c r="F64" s="14"/>
       <c r="G64" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H64" s="31" t="s">
+      <c r="H64" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I64" s="28"/>
+      <c r="I64" s="19"/>
     </row>
     <row r="65" spans="2:9">
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="18" t="s">
+      <c r="C65" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="20">
+      <c r="D65" s="14">
         <v>10</v>
       </c>
-      <c r="E65" s="20" t="s">
+      <c r="E65" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F65" s="20"/>
+      <c r="F65" s="14"/>
       <c r="G65" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H65" s="29"/>
-      <c r="I65" s="28"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="19"/>
     </row>
     <row r="66" spans="2:9">
-      <c r="B66" s="14"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="11"/>
+      <c r="H66" s="5"/>
       <c r="I66" s="2"/>
     </row>
     <row r="67" spans="2:9" ht="17" thickBot="1">
-      <c r="B67" s="15"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
       <c r="G67" s="3"/>
-      <c r="H67" s="12"/>
+      <c r="H67" s="6"/>
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="2:9" ht="17" thickTop="1"/>
     <row r="70" spans="2:9" ht="17" thickBot="1"/>
     <row r="71" spans="2:9" ht="17" thickTop="1">
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="8" t="s">
+      <c r="C71" s="27"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="10"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="31"/>
     </row>
     <row r="72" spans="2:9">
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="18" t="s">
+      <c r="C72" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="20" t="s">
+      <c r="D72" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E72" s="20" t="s">
+      <c r="E72" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F72" s="22" t="s">
+      <c r="F72" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H72" s="11" t="s">
+      <c r="H72" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I72" s="2" t="s">
@@ -1683,97 +1691,97 @@
       </c>
     </row>
     <row r="73" spans="2:9">
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D73" s="20">
+      <c r="D73" s="14">
         <v>10</v>
       </c>
-      <c r="E73" s="20" t="s">
+      <c r="E73" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F73" s="20"/>
+      <c r="F73" s="14"/>
       <c r="G73" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H73" s="11"/>
+      <c r="H73" s="5"/>
       <c r="I73" s="2"/>
     </row>
     <row r="74" spans="2:9">
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C74" s="18" t="s">
+      <c r="C74" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D74" s="20">
+      <c r="D74" s="14">
         <v>100</v>
       </c>
-      <c r="E74" s="20" t="s">
+      <c r="E74" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F74" s="20" t="s">
+      <c r="F74" s="14" t="s">
         <v>39</v>
       </c>
       <c r="G74" s="1"/>
-      <c r="H74" s="11"/>
+      <c r="H74" s="5"/>
       <c r="I74" s="2"/>
     </row>
     <row r="75" spans="2:9">
-      <c r="B75" s="14"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
       <c r="G75" s="1"/>
-      <c r="H75" s="11"/>
+      <c r="H75" s="5"/>
       <c r="I75" s="2"/>
     </row>
     <row r="76" spans="2:9" ht="17" thickBot="1">
-      <c r="B76" s="15"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="21"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
       <c r="G76" s="3"/>
-      <c r="H76" s="12"/>
+      <c r="H76" s="6"/>
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="2:9" ht="17" thickTop="1"/>
     <row r="79" spans="2:9" ht="17" thickBot="1"/>
     <row r="80" spans="2:9" ht="17" thickTop="1">
-      <c r="B80" s="5"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="10"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="30"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="31"/>
     </row>
     <row r="81" spans="2:9">
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C81" s="18" t="s">
+      <c r="C81" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="20" t="s">
+      <c r="D81" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E81" s="20" t="s">
+      <c r="E81" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F81" s="22" t="s">
+      <c r="F81" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H81" s="11" t="s">
+      <c r="H81" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I81" s="2" t="s">
@@ -1781,81 +1789,81 @@
       </c>
     </row>
     <row r="82" spans="2:9">
-      <c r="B82" s="14"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
       <c r="G82" s="1"/>
-      <c r="H82" s="11"/>
+      <c r="H82" s="5"/>
       <c r="I82" s="2"/>
     </row>
     <row r="83" spans="2:9">
-      <c r="B83" s="14"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
       <c r="G83" s="1"/>
-      <c r="H83" s="11"/>
+      <c r="H83" s="5"/>
       <c r="I83" s="2"/>
     </row>
     <row r="84" spans="2:9">
-      <c r="B84" s="14"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
       <c r="G84" s="1"/>
-      <c r="H84" s="11"/>
+      <c r="H84" s="5"/>
       <c r="I84" s="2"/>
     </row>
     <row r="85" spans="2:9" ht="17" thickBot="1">
-      <c r="B85" s="15"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="12"/>
+      <c r="H85" s="6"/>
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="2:9" ht="17" thickTop="1"/>
     <row r="91" spans="2:9" ht="17" thickBot="1"/>
     <row r="92" spans="2:9" ht="17" thickTop="1">
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C92" s="6"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="8" t="s">
+      <c r="C92" s="27"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-      <c r="I92" s="10"/>
+      <c r="F92" s="30"/>
+      <c r="G92" s="30"/>
+      <c r="H92" s="30"/>
+      <c r="I92" s="31"/>
     </row>
     <row r="93" spans="2:9">
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C93" s="18" t="s">
+      <c r="C93" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="20" t="s">
+      <c r="D93" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E93" s="20" t="s">
+      <c r="E93" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F93" s="22" t="s">
+      <c r="F93" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H93" s="11" t="s">
+      <c r="H93" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I93" s="2" t="s">
@@ -1863,54 +1871,48 @@
       </c>
     </row>
     <row r="94" spans="2:9">
-      <c r="B94" s="14"/>
-      <c r="C94" s="18"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
       <c r="G94" s="1"/>
-      <c r="H94" s="11"/>
+      <c r="H94" s="5"/>
       <c r="I94" s="2"/>
     </row>
     <row r="95" spans="2:9">
-      <c r="B95" s="14"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
       <c r="G95" s="1"/>
-      <c r="H95" s="11"/>
+      <c r="H95" s="5"/>
       <c r="I95" s="2"/>
     </row>
     <row r="96" spans="2:9">
-      <c r="B96" s="14"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
       <c r="G96" s="1"/>
-      <c r="H96" s="11"/>
+      <c r="H96" s="5"/>
       <c r="I96" s="2"/>
     </row>
     <row r="97" spans="2:9" ht="17" thickBot="1">
-      <c r="B97" s="15"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="21"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
       <c r="G97" s="3"/>
-      <c r="H97" s="12"/>
+      <c r="H97" s="6"/>
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="2:9" ht="17" thickTop="1"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="E92:I92"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="E80:I80"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="E71:I71"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:I62"/>
     <mergeCell ref="H64:H65"/>
@@ -1922,6 +1924,12 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:I21"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="E92:I92"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="E80:I80"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="E71:I71"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>